<commit_message>
use uinode ,rather than gameobject to record parent
</commit_message>
<xml_diff>
--- a/UI命名.xlsx
+++ b/UI命名.xlsx
@@ -418,6 +418,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,24 +453,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -738,7 +738,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -751,7 +751,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -763,22 +763,22 @@
       <c r="D1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
@@ -786,13 +786,13 @@
       <c r="E2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
@@ -801,13 +801,13 @@
         <v>39</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -816,13 +816,13 @@
         <v>36</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
@@ -831,13 +831,13 @@
         <v>37</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="6" t="s">
         <v>28</v>
       </c>
@@ -847,16 +847,16 @@
       <c r="D6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
@@ -867,10 +867,10 @@
         <v>43</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
@@ -884,10 +884,10 @@
         <v>43</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -899,10 +899,10 @@
         <v>48</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -914,10 +914,10 @@
         <v>46</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
@@ -928,13 +928,13 @@
         <v>47</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
@@ -942,7 +942,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -951,11 +951,11 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="21"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -967,20 +967,20 @@
       <c r="D14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="15" t="s">
+      <c r="F14" s="14"/>
+      <c r="G14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
@@ -993,13 +993,13 @@
       <c r="E15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
@@ -1012,13 +1012,13 @@
       <c r="E16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1031,67 +1031,67 @@
       <c r="E17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="21"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="21"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="21"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="21"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="21"/>
+      <c r="F22" s="15"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="15"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
no matter handle visiable or not,slider will be supported
</commit_message>
<xml_diff>
--- a/UI命名.xlsx
+++ b/UI命名.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>控件类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -247,12 +247,28 @@
     <t>V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>PSDName.xml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>带Globle名的xml，会将图片导入到指定文件夹中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b_,h_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,8 +308,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +346,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -384,11 +413,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -454,10 +486,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="好" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -735,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -859,7 +893,9 @@
       <c r="E6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
@@ -873,10 +909,12 @@
         <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="15"/>
+      <c r="F7" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
@@ -893,7 +931,9 @@
         <v>38</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
@@ -1103,6 +1143,14 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
add support to inputfield
</commit_message>
<xml_diff>
--- a/UI命名.xlsx
+++ b/UI命名.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>控件类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,10 +181,6 @@
   </si>
   <si>
     <t>l,r,t,b</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b_,t_,h_</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -261,6 +257,14 @@
   </si>
   <si>
     <t>b_,h_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b_,t_,h_</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -468,6 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -486,7 +491,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -772,7 +776,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -786,7 +790,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -802,34 +806,34 @@
         <v>31</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+        <v>46</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="20"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+        <v>47</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
@@ -839,14 +843,14 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+        <v>47</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -856,14 +860,14 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
+        <v>47</v>
+      </c>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
@@ -873,14 +877,14 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+        <v>47</v>
+      </c>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="6" t="s">
         <v>25</v>
       </c>
@@ -891,17 +895,17 @@
         <v>35</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+        <v>50</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="6" t="s">
         <v>27</v>
       </c>
@@ -909,15 +913,15 @@
         <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+        <v>50</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
@@ -932,11 +936,11 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
+        <v>50</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -945,13 +949,13 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -960,13 +964,15 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
+      <c r="F10" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
@@ -974,16 +980,16 @@
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="15"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
@@ -1004,7 +1010,7 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1020,16 +1026,16 @@
         <v>9</v>
       </c>
       <c r="F14" s="14"/>
-      <c r="G14" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
+      <c r="G14" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
@@ -1042,13 +1048,15 @@
       <c r="E15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
+      <c r="F15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
     </row>
     <row r="16" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
@@ -1061,13 +1069,15 @@
       <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
+      <c r="F16" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
     </row>
     <row r="17" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1080,13 +1090,15 @@
       <c r="E17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
+      <c r="F17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1095,7 +1107,7 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1104,7 +1116,7 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1113,7 +1125,7 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1122,18 +1134,20 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="15"/>
+      <c r="F22" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1146,10 +1160,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add grid support, get return value function to layerImport
</commit_message>
<xml_diff>
--- a/UI命名.xlsx
+++ b/UI命名.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>控件类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,10 +122,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>滑动区@ScrollView</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>滑动条@Slider</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -181,10 +177,6 @@
   </si>
   <si>
     <t>l,r,t,b</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v,h,vh;0-N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -265,6 +257,26 @@
   </si>
   <si>
     <t>b_,t_,h_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格子@Grid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v,h;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> @Size (小格子的尺寸)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c,r;1-n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>滑动区@ScrollView</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -424,7 +436,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -473,6 +485,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -773,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -790,7 +803,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -800,209 +813,215 @@
         <v>23</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+        <v>44</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+        <v>45</v>
+      </c>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+        <v>45</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+        <v>45</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+        <v>45</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="22"/>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
+        <v>48</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+        <v>48</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+        <v>50</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F11" s="15"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F12" s="15"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1010,122 +1029,104 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
+      <c r="F14" s="18"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="3" t="s">
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-    </row>
-    <row r="16" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="3" t="s">
+      <c r="F18" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-    </row>
-    <row r="17" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="3" t="s">
+      <c r="F19" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="1"/>
+      <c r="F20" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1134,20 +1135,16 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="A22" s="20"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="F22" s="15"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1156,21 +1153,52 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>49</v>
+      <c r="A25" s="20"/>
+      <c r="B25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="20"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A14:A23"/>
+    <mergeCell ref="A17:A26"/>
     <mergeCell ref="A1:A7"/>
-    <mergeCell ref="G14:I17"/>
+    <mergeCell ref="G17:I20"/>
     <mergeCell ref="G1:I11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1184,8 +1212,9 @@
     <hyperlink ref="B9" r:id="rId7"/>
     <hyperlink ref="B10" r:id="rId8"/>
     <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add support to Group(vertical ,horizontal)
</commit_message>
<xml_diff>
--- a/UI命名.xlsx
+++ b/UI命名.xlsx
@@ -251,10 +251,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>v,h;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>c,r;1-n</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -275,10 +271,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> @Size（有背景可不写）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> @Size (小格子的尺寸)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -292,6 +284,14 @@
   </si>
   <si>
     <t>c_,vb_,hb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v,h;0-n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -497,6 +497,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -514,9 +517,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -803,7 +803,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -817,7 +817,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -830,40 +830,40 @@
         <v>32</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="20"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="23" t="s">
         <v>54</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
@@ -875,12 +875,12 @@
       <c r="F3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -892,12 +892,12 @@
       <c r="F4" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
@@ -909,33 +909,33 @@
       <c r="F5" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="6" t="s">
         <v>26</v>
       </c>
@@ -949,9 +949,9 @@
       <c r="F7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
@@ -968,9 +968,9 @@
       <c r="F8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -983,9 +983,9 @@
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -1000,9 +1000,9 @@
       <c r="F10" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
@@ -1010,16 +1010,16 @@
         <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+      <c r="F11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
@@ -1027,14 +1027,14 @@
         <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1059,7 +1059,7 @@
       <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1075,14 +1075,14 @@
         <v>9</v>
       </c>
       <c r="F17" s="12"/>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -1098,12 +1098,12 @@
       <c r="F18" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -1119,12 +1119,12 @@
       <c r="F19" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1140,12 +1140,12 @@
       <c r="F20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1154,7 +1154,7 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1163,7 +1163,7 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1172,7 +1172,7 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1181,7 +1181,7 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="5" t="s">
         <v>13</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>

</xml_diff>

<commit_message>
full support to dropdown
</commit_message>
<xml_diff>
--- a/UI命名.xlsx
+++ b/UI命名.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>控件类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,10 +130,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>下拉框@DropDown</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>输入框@InputField</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -172,10 +168,6 @@
   </si>
   <si>
     <t>l,r,t,b</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b_,a_,l_,t_,tb_,ta,tl_</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -292,6 +284,22 @@
   </si>
   <si>
     <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b1_,b2_,b3,l1_,l2,m_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下拉框@Dropdown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vb_</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -802,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -827,16 +835,16 @@
         <v>23</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
@@ -850,13 +858,13 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
@@ -869,11 +877,11 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
@@ -886,11 +894,11 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
@@ -903,11 +911,11 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -916,19 +924,19 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="B6" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
@@ -940,14 +948,14 @@
         <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -959,14 +967,14 @@
         <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
@@ -975,14 +983,18 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="6" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="13"/>
+        <v>59</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
@@ -990,15 +1002,15 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
@@ -1007,15 +1019,15 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="16"/>
       <c r="F11" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
@@ -1024,17 +1036,17 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1076,7 +1088,7 @@
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
@@ -1096,7 +1108,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
@@ -1117,7 +1129,7 @@
         <v>22</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
@@ -1138,7 +1150,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
@@ -1189,7 +1201,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1207,10 +1219,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>